<commit_message>
✨ (Error handling) - Improve error handling
</commit_message>
<xml_diff>
--- a/src/constant/_SIREN.xlsx
+++ b/src/constant/_SIREN.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\DEV\Projet_perso\sirene-api-project\src\constant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A10856-AA1D-4019-9815-52FB41D46BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDB8778-1738-4034-88E6-AECFA33CFB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{AB59BD47-33AD-4FD4-AE4D-454350B9D8D0}"/>
+    <workbookView xWindow="6000" yWindow="1635" windowWidth="18000" windowHeight="9360" xr2:uid="{AB59BD47-33AD-4FD4-AE4D-454350B9D8D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
     <definedName name="Segment_DEPARTEMENT">#N/A</definedName>
   </definedNames>
@@ -25,7 +28,7 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
       <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicerCache r:id="rId2"/>
+        <x14:slicerCache r:id="rId3"/>
       </x15:slicerCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>NOM</t>
   </si>
@@ -120,6 +123,24 @@
   </si>
   <si>
     <t>DEPARTEMENT</t>
+  </si>
+  <si>
+    <t>ATELIERS PERRAULT FRERES</t>
+  </si>
+  <si>
+    <t>MAUGES-SUR-LOIRE</t>
+  </si>
+  <si>
+    <t>COMEC</t>
+  </si>
+  <si>
+    <t>LA TESSOUALLE</t>
+  </si>
+  <si>
+    <t>DEPANN' RENOV</t>
+  </si>
+  <si>
+    <t>ANGERS</t>
   </si>
 </sst>
 </file>
@@ -155,8 +176,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,6 +283,22 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Feuil1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Segment_DEPARTEMENT" xr10:uid="{76230500-43F2-4597-A874-9080E0D0E3B8}" sourceName="DEPARTEMENT">
   <extLst>
@@ -278,8 +316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D74ACC76-F182-4E8C-BAC4-D9D74DC9DE53}" name="Tableau1" displayName="Tableau1" ref="A1:E11" totalsRowShown="0">
-  <autoFilter ref="A1:E11" xr:uid="{D74ACC76-F182-4E8C-BAC4-D9D74DC9DE53}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D74ACC76-F182-4E8C-BAC4-D9D74DC9DE53}" name="Tableau1" displayName="Tableau1" ref="A1:E14" totalsRowShown="0">
+  <autoFilter ref="A1:E14" xr:uid="{D74ACC76-F182-4E8C-BAC4-D9D74DC9DE53}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{866143AD-F8B3-4A0B-8437-8F3B4671E2B1}" name="NOM"/>
     <tableColumn id="2" xr3:uid="{3C593F94-D569-48DE-916F-985D1799B69C}" name="VILLE"/>
@@ -588,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115FDEB7-E900-472E-954B-5CAB04EF6E35}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,6 +836,60 @@
       </c>
       <c r="E11">
         <v>842099913</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>49110</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f>LEFT([1]!Tableau1[[#This Row],[CODE POSTAL]],2)</f>
+        <v>44</v>
+      </c>
+      <c r="E12">
+        <v>61201083</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>49280</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f>LEFT([1]!Tableau1[[#This Row],[CODE POSTAL]],2)</f>
+        <v>44</v>
+      </c>
+      <c r="E13">
+        <v>61200226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>49100</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f>LEFT([1]!Tableau1[[#This Row],[CODE POSTAL]],2)</f>
+        <v>44</v>
+      </c>
+      <c r="E14">
+        <v>882857782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>